<commit_message>
From 0.1 to 1.0 version
</commit_message>
<xml_diff>
--- a/output/xlsx/RF001 - Autenticar Usuario--ART-.xlsx
+++ b/output/xlsx/RF001 - Autenticar Usuario--ART-.xlsx
@@ -32,7 +32,7 @@
     <t xml:space="preserve">Version: </t>
   </si>
   <si>
-    <t>0.1</t>
+    <t>1.0</t>
   </si>
   <si>
     <t>Suite Type:</t>
@@ -92,7 +92,7 @@
     <t>Actual Result</t>
   </si>
   <si>
-    <t>Usuario do Sistema inicia a tela de login atraves da opcao de login no canto superior direito</t>
+    <t>Usuario do Sistema inicia a tela de login atraves da opcao de Login no canto superior direito</t>
   </si>
   <si>
     <t>SYSTEM apresenta um formulario com campos de nome de usuario e senha e um botao entrar</t>

</xml_diff>